<commit_message>
Implementacion de tabulate en def listarProductos
</commit_message>
<xml_diff>
--- a/backend/datos.xlsx
+++ b/backend/datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billbravo/Code/upb/bragar/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f557778394dfb93a/Escritorio/bragar/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0A80C5-38F1-4548-8488-80F4D731A384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{6D0A80C5-38F1-4548-8488-80F4D731A384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3446087B-32A1-448E-AE42-4518FFE5607A}"/>
   <bookViews>
-    <workbookView xWindow="17840" yWindow="4400" windowWidth="28040" windowHeight="17440" xr2:uid="{BAEA4CE5-C3D3-7C47-816C-2C82F69F15A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BAEA4CE5-C3D3-7C47-816C-2C82F69F15A2}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
@@ -36,36 +36,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Número de documento</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Jose Luis</t>
-  </si>
-  <si>
-    <t>Juan de Dios</t>
-  </si>
-  <si>
-    <t>Medellín</t>
-  </si>
-  <si>
-    <t>Cali</t>
-  </si>
-  <si>
     <t>1101</t>
   </si>
   <si>
     <t>1203</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Macbook air M3</t>
+  </si>
+  <si>
+    <t>Macbook Pro M4</t>
+  </si>
+  <si>
+    <t>2000$</t>
+  </si>
+  <si>
+    <t>1000$</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -122,7 +128,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -440,58 +446,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777A22BA-72E6-5540-B074-CAB76FCB2FF4}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1">
-        <v>3002345678</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3105439876</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funcion crearProducto y eliminarProducto
</commit_message>
<xml_diff>
--- a/backend/datos.xlsx
+++ b/backend/datos.xlsx
@@ -1,95 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f557778394dfb93a/Escritorio/bragar/backend/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{6D0A80C5-38F1-4548-8488-80F4D731A384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3446087B-32A1-448E-AE42-4518FFE5607A}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BAEA4CE5-C3D3-7C47-816C-2C82F69F15A2}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="clientes" sheetId="1" r:id="rId1"/>
+    <sheet name="clientes" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>1101</t>
-  </si>
-  <si>
-    <t>1203</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>Macbook air M3</t>
-  </si>
-  <si>
-    <t>Macbook Pro M4</t>
-  </si>
-  <si>
-    <t>2000$</t>
-  </si>
-  <si>
-    <t>1000$</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -443,61 +440,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777A22BA-72E6-5540-B074-CAB76FCB2FF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.796875" style="1"/>
+    <col width="12.19921875" customWidth="1" style="1" min="1" max="1"/>
+    <col width="15.59765625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="11.19921875" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="10.796875" customWidth="1" style="1" min="4" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Precio</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cantidad</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>1203</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Macbook Pro M4</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>2000$</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Producto A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funcion frontend agregaProducto, eliminarProducto. Implementamos en mostrarMenuProducto
</commit_message>
<xml_diff>
--- a/backend/datos.xlsx
+++ b/backend/datos.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -525,6 +525,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>12314</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12313</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>12313</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se implementa la opción de actualizar producto
</commit_message>
<xml_diff>
--- a/backend/datos.xlsx
+++ b/backend/datos.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="21940" yWindow="2280" windowWidth="23260" windowHeight="13180" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="clientes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="productos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -445,18 +445,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col width="12.19921875" customWidth="1" style="1" min="1" max="1"/>
-    <col width="15.59765625" customWidth="1" style="1" min="2" max="2"/>
-    <col width="11.19921875" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
-    <col width="10.796875" customWidth="1" style="1" min="4" max="16384"/>
+    <col width="12.1640625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="15.6640625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="11.1640625" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="10.83203125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="10.83203125" customWidth="1" style="1" min="5" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -484,7 +485,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>1203</t>
+          <t>1201</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -504,9 +505,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>12345</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>1202</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -522,6 +523,28 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1203</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>iPhone 16 Pro</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>999</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>

</xml_diff>